<commit_message>
Move to jars to maven dependencies
</commit_message>
<xml_diff>
--- a/examples/template_out.xlsx
+++ b/examples/template_out.xlsx
@@ -469,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>42395.42180689815</v>
+        <v>42395.4452893287</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -477,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>27.0</v>
+        <v>70.0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>